<commit_message>
导入导出忽略 tenant_id, tenant_id_lbl 等
</commit_message>
<xml_diff>
--- a/codegen/__out__/pc/public/excel_template/base/dictbiz.xlsx
+++ b/codegen/__out__/pc/public/excel_template/base/dictbiz.xlsx
@@ -60,9 +60,6 @@
     <t xml:space="preserve">&lt;%=comment.update_usr_id_lbl%&gt;&lt;%selectList.update_usr_id = data.findAllUsr.map((item) =&gt; item.lbl)%&gt;&lt;%_dataValidation_({ sqref: `${ _col }2:${ _col }${ _lastRow }`, formula1: `"${ selectList.update_usr_id.join(",") }"` })%&gt;</t>
   </si>
   <si>
-    <t xml:space="preserve">&lt;%=comment.tenant_id_lbl%&gt;&lt;%selectList.tenant_id = data.findAllTenant.map((item) =&gt; item.lbl)%&gt;&lt;%_dataValidation_({ sqref: `${ _col }2:${ _col }${ _lastRow }`, formula1: `"${ selectList.tenant_id.join(",") }"` })%&gt;</t>
-  </si>
-  <si>
     <t xml:space="preserve">&lt;%=comment.update_time_lbl%&gt;</t>
   </si>
   <si>
@@ -94,9 +91,6 @@
   </si>
   <si>
     <t xml:space="preserve">&lt;%=model.update_usr_id_lbl%&gt;</t>
-  </si>
-  <si>
-    <t xml:space="preserve">&lt;%=model.tenant_id_lbl%&gt;</t>
   </si>
   <si>
     <t xml:space="preserve">&lt;%~model.update_time ? new Date(model.update_time) : ""%&gt;</t>
@@ -464,46 +458,40 @@
       <c r="K1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
-        <v>11</v>
-      </c>
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.4">
       <c r="A2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" t="s">
         <v>12</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>13</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>14</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>15</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>16</v>
       </c>
-      <c r="F2" t="s">
+      <c r="G2" t="s">
         <v>17</v>
       </c>
-      <c r="G2" t="s">
+      <c r="H2" t="s">
         <v>18</v>
       </c>
-      <c r="H2" t="s">
+      <c r="I2" t="s">
         <v>19</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>20</v>
       </c>
-      <c r="J2" t="s">
+      <c r="K2" t="s">
         <v>21</v>
-      </c>
-      <c r="K2" t="s">
-        <v>22</v>
-      </c>
-      <c r="L2" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>